<commit_message>
Added SIE-VAST - partner for Bidoup plot
</commit_message>
<xml_diff>
--- a/ForestGEO Partners.xlsx
+++ b/ForestGEO Partners.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartdavies/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krizell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="460" windowWidth="25440" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15800" windowHeight="6650" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>LIST OF FORESTGEO PARTNERS</t>
   </si>
@@ -264,12 +264,15 @@
   </si>
   <si>
     <t xml:space="preserve">Centre de Formation et de Recherche en Conservation Foresti ere (CEFRECOF) Epulu, Ituri Forest, Reserve de Faune a Okapis, Epulu, Democratic Republic of Congo </t>
+  </si>
+  <si>
+    <t>Southern Institute of Ecology, Vietnam Academy of Science and Technology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -325,6 +328,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -593,411 +599,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A79"/>
+  <dimension ref="A1:A80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="54.5" style="1" customWidth="1"/>
     <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>